<commit_message>
COMMIT DE LA S_16
EVAL CREER LA BDD TERMINEE. PARTIE NOSQL FAITE.
</commit_message>
<xml_diff>
--- a/S_16/Annexe 3 Programme hebdo de travail.xlsx
+++ b/S_16/Annexe 3 Programme hebdo de travail.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24020"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\80010-48-01\Desktop\DWWM\S_15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\80010-48-01\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96804F13-28FC-46DB-A134-58792E7E6A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil2" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>PROGRAMME HEBDOMADAIRE DE TRAVAIL (des activités réalisées à distance)</t>
   </si>
@@ -41,10 +42,16 @@
     <t xml:space="preserve">formation : </t>
   </si>
   <si>
+    <t>DWWM</t>
+  </si>
+  <si>
     <t xml:space="preserve">offre n° : </t>
   </si>
   <si>
     <t xml:space="preserve">nom/prenom stagiaire : </t>
+  </si>
+  <si>
+    <t>GUEULLE Matthieu</t>
   </si>
   <si>
     <t>Mois</t>
@@ -105,50 +112,110 @@
     <t>Créer la BDD</t>
   </si>
   <si>
-    <t>MCD Merise</t>
-  </si>
-  <si>
-    <t>cas Note</t>
-  </si>
-  <si>
-    <t>cas_note.loo</t>
-  </si>
-  <si>
-    <t>DWWM/S_15</t>
+    <t>Oto</t>
+  </si>
+  <si>
+    <t>Alimenter la BDD</t>
+  </si>
+  <si>
+    <t>Exo 2</t>
+  </si>
+  <si>
+    <t>exercice_2.txt</t>
+  </si>
+  <si>
+    <t>DWWM/S_16/alimenter_la_bdd</t>
   </si>
   <si>
     <t>Github</t>
   </si>
   <si>
-    <t>cas Blog</t>
-  </si>
-  <si>
-    <t>cas_blog.loo</t>
-  </si>
-  <si>
-    <t>cas Gescom</t>
-  </si>
-  <si>
-    <t>cas_gescom.loo</t>
-  </si>
-  <si>
-    <t>Oto</t>
-  </si>
-  <si>
-    <t>DWWM</t>
-  </si>
-  <si>
-    <t>GUEULLE MATTHIEU</t>
+    <t>Exo 4</t>
+  </si>
+  <si>
+    <t>orders_details.csv</t>
+  </si>
+  <si>
+    <t>Exo 5</t>
+  </si>
+  <si>
+    <t>exercice_5.sql ; exercice_5_entrees.sql</t>
+  </si>
+  <si>
+    <t>Interroger la BDD</t>
+  </si>
+  <si>
+    <t>DWWM/S_16/interroger_la_bdd</t>
+  </si>
+  <si>
+    <t>20-21</t>
+  </si>
+  <si>
+    <t>EVAL 4.Interroger la BDD</t>
+  </si>
+  <si>
+    <t>gescom_afpa_requetes.sql</t>
+  </si>
+  <si>
+    <t>Utilisateurs, privilèges et rôles</t>
+  </si>
+  <si>
+    <t>Exo création util1, 2 et 3</t>
+  </si>
+  <si>
+    <t>utilisateurs_gescom.sql</t>
+  </si>
+  <si>
+    <t>DWWM/S_16/utilisateurs_privileges_roles</t>
+  </si>
+  <si>
+    <t>EVAL 5. Rôles</t>
+  </si>
+  <si>
+    <t>r_marketing_gescom.sql</t>
+  </si>
+  <si>
+    <t>Assurer les sauvegardes</t>
+  </si>
+  <si>
+    <t>EVAL 6. Assurer les sauvegardes</t>
+  </si>
+  <si>
+    <t>backup_afpa_gescom.sql</t>
+  </si>
+  <si>
+    <t>DWWM/S_16/assurer_les_sauvegardes/Backup</t>
+  </si>
+  <si>
+    <t>Bases de données NoSQL</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>questions.txt</t>
+  </si>
+  <si>
+    <t>DWWM/S_16/bases_de_donnees_nosql</t>
+  </si>
+  <si>
+    <t>Pratique de MongoDB</t>
+  </si>
+  <si>
+    <t>script_mongodb.sql</t>
+  </si>
+  <si>
+    <t>DWWM/S_16/bases_de_donnees_nosql/pratique_mongodb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -709,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -759,13 +826,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1217,34 +1288,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19:L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18.75">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="18.75">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
@@ -1253,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="3"/>
@@ -1263,13 +1334,13 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18.75">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="F4" s="23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="4"/>
@@ -1280,17 +1351,17 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="22.5">
       <c r="A5" s="1"/>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
@@ -1300,7 +1371,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="19.5" thickBot="1">
       <c r="A6" s="1"/>
       <c r="B6" s="6"/>
       <c r="C6" s="7"/>
@@ -1316,339 +1387,445 @@
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="46" t="s">
+    <row r="7" spans="1:14" ht="14.45" customHeight="1">
+      <c r="A7" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="B7" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="C7" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="52"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="64" t="s">
+      <c r="D7" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="49" t="s">
+      <c r="E7" s="53" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="55"/>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="56"/>
-      <c r="J8" s="58" t="s">
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="59"/>
-      <c r="L8" s="60" t="s">
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="62" t="s">
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="43"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="50"/>
-    </row>
-    <row r="9" spans="1:14" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="42"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="50"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="62" t="s">
+        <v>14</v>
+      </c>
+      <c r="M8" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="52"/>
+    </row>
+    <row r="9" spans="1:14" ht="90">
+      <c r="A9" s="44"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="52"/>
       <c r="E9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="25" t="s">
+      <c r="F9" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="G9" s="28" t="s">
         <v>18</v>
       </c>
+      <c r="H9" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>20</v>
+      </c>
       <c r="J9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="63"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="52"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="36">
+        <v>16</v>
+      </c>
+      <c r="C10" s="19">
         <v>19</v>
       </c>
-      <c r="K9" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="61"/>
-      <c r="M9" s="63"/>
-      <c r="N9" s="50"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="34">
-        <v>15</v>
-      </c>
-      <c r="C10" s="19">
-        <v>12</v>
-      </c>
       <c r="D10" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
+        <v>24</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="21">
+        <v>1</v>
+      </c>
       <c r="H10" s="21"/>
-      <c r="I10" s="22"/>
+      <c r="I10" s="26">
+        <v>44305</v>
+      </c>
       <c r="J10" s="20"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
       <c r="M10" s="22"/>
       <c r="N10" s="19"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="38"/>
-      <c r="B11" s="35"/>
+    <row r="11" spans="1:14">
+      <c r="A11" s="40"/>
+      <c r="B11" s="37"/>
       <c r="C11" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G11" s="11">
         <v>1</v>
       </c>
       <c r="H11" s="11"/>
-      <c r="I11" s="27">
-        <v>44299</v>
+      <c r="I11" s="25">
+        <v>44306</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M11" s="15"/>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="12">
-        <v>14</v>
-      </c>
+    <row r="12" spans="1:14">
+      <c r="A12" s="40"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G12" s="11">
         <v>1</v>
       </c>
       <c r="H12" s="11"/>
-      <c r="I12" s="27">
-        <v>44300</v>
+      <c r="I12" s="25">
+        <v>44306</v>
       </c>
       <c r="J12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="11" t="s">
-        <v>26</v>
-      </c>
       <c r="L12" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="12">
-        <v>15</v>
-      </c>
+    <row r="13" spans="1:14">
+      <c r="A13" s="40"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G13" s="11">
         <v>1</v>
       </c>
       <c r="H13" s="11"/>
-      <c r="I13" s="27">
-        <v>44301</v>
+      <c r="I13" s="25">
+        <v>44306</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="L13" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="M13" s="15"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="12">
-        <v>16</v>
-      </c>
+    <row r="14" spans="1:14">
+      <c r="A14" s="40"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="12"/>
       <c r="D14" s="19" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>32</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F14" s="11"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="25">
+        <v>44306</v>
+      </c>
       <c r="J14" s="14"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
+      <c r="K14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="M14" s="15"/>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="38"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+    <row r="15" spans="1:14">
+      <c r="A15" s="40"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
       <c r="H15" s="11"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
+      <c r="I15" s="25">
+        <v>44307</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="M15" s="15"/>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="38"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+    <row r="16" spans="1:14">
+      <c r="A16" s="40"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="12">
+        <v>22</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="11">
+        <v>1</v>
+      </c>
       <c r="H16" s="11"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
+      <c r="I16" s="25">
+        <v>44308</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="M16" s="15"/>
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="38"/>
-      <c r="B17" s="35"/>
+    <row r="17" spans="1:14">
+      <c r="A17" s="40"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="D17" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="11">
+        <v>1</v>
+      </c>
       <c r="H17" s="11"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="15"/>
+      <c r="I17" s="25">
+        <v>44308</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="11"/>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="35"/>
+    <row r="18" spans="1:14">
+      <c r="A18" s="40"/>
+      <c r="B18" s="37"/>
       <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="D18" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="11">
+        <v>1</v>
+      </c>
       <c r="H18" s="11"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
+      <c r="I18" s="25">
+        <v>44308</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="M18" s="15"/>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="38"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+    <row r="19" spans="1:14">
+      <c r="A19" s="40"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="12">
+        <v>23</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="11">
+        <v>1</v>
+      </c>
       <c r="H19" s="11"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="I19" s="25">
+        <v>44309</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="L19" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="M19" s="15"/>
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
+    <row r="20" spans="1:14">
+      <c r="A20" s="40"/>
+      <c r="B20" s="37"/>
       <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="D20" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="11">
+        <v>1</v>
+      </c>
       <c r="H20" s="11"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
+      <c r="I20" s="25">
+        <v>44309</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="M20" s="15"/>
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="38"/>
-      <c r="B21" s="35"/>
+    <row r="21" spans="1:14">
+      <c r="A21" s="40"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="14"/>
@@ -1662,9 +1839,9 @@
       <c r="M21" s="15"/>
       <c r="N21" s="12"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="38"/>
-      <c r="B22" s="35"/>
+    <row r="22" spans="1:14">
+      <c r="A22" s="40"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="14"/>
@@ -1678,9 +1855,9 @@
       <c r="M22" s="15"/>
       <c r="N22" s="12"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="38"/>
-      <c r="B23" s="35"/>
+    <row r="23" spans="1:14">
+      <c r="A23" s="40"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="14"/>
@@ -1694,9 +1871,9 @@
       <c r="M23" s="15"/>
       <c r="N23" s="12"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="38"/>
-      <c r="B24" s="35"/>
+    <row r="24" spans="1:14">
+      <c r="A24" s="40"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="14"/>
@@ -1710,9 +1887,9 @@
       <c r="M24" s="15"/>
       <c r="N24" s="12"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="38"/>
-      <c r="B25" s="35"/>
+    <row r="25" spans="1:14">
+      <c r="A25" s="40"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="14"/>
@@ -1726,9 +1903,9 @@
       <c r="M25" s="15"/>
       <c r="N25" s="12"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="38"/>
-      <c r="B26" s="35"/>
+    <row r="26" spans="1:14">
+      <c r="A26" s="40"/>
+      <c r="B26" s="37"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="14"/>
@@ -1742,9 +1919,9 @@
       <c r="M26" s="15"/>
       <c r="N26" s="12"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="38"/>
-      <c r="B27" s="35"/>
+    <row r="27" spans="1:14">
+      <c r="A27" s="40"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="14"/>
@@ -1758,9 +1935,9 @@
       <c r="M27" s="15"/>
       <c r="N27" s="12"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="38"/>
-      <c r="B28" s="35"/>
+    <row r="28" spans="1:14">
+      <c r="A28" s="40"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="14"/>
@@ -1774,9 +1951,9 @@
       <c r="M28" s="15"/>
       <c r="N28" s="12"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
-      <c r="B29" s="35"/>
+    <row r="29" spans="1:14">
+      <c r="A29" s="40"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="14"/>
@@ -1790,9 +1967,9 @@
       <c r="M29" s="15"/>
       <c r="N29" s="12"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="38"/>
-      <c r="B30" s="35"/>
+    <row r="30" spans="1:14">
+      <c r="A30" s="40"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="14"/>
@@ -1806,26 +1983,26 @@
       <c r="M30" s="15"/>
       <c r="N30" s="12"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="39"/>
-      <c r="B31" s="36"/>
+    <row r="31" spans="1:14">
+      <c r="A31" s="41"/>
+      <c r="B31" s="38"/>
       <c r="C31" s="13"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="18"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
       <c r="N31" s="13"/>
     </row>
-    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="31"/>
+    <row r="32" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="33" spans="1:14">
+      <c r="A33" s="30"/>
+      <c r="B33" s="33"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
       <c r="E33" s="20"/>
@@ -1839,9 +2016,9 @@
       <c r="M33" s="22"/>
       <c r="N33" s="19"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="32"/>
+    <row r="34" spans="1:14">
+      <c r="A34" s="31"/>
+      <c r="B34" s="34"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="14"/>
@@ -1855,9 +2032,9 @@
       <c r="M34" s="15"/>
       <c r="N34" s="12"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="32"/>
+    <row r="35" spans="1:14">
+      <c r="A35" s="31"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="14"/>
@@ -1871,9 +2048,9 @@
       <c r="M35" s="15"/>
       <c r="N35" s="12"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="32"/>
+    <row r="36" spans="1:14">
+      <c r="A36" s="31"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="14"/>
@@ -1887,9 +2064,9 @@
       <c r="M36" s="15"/>
       <c r="N36" s="12"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="32"/>
+    <row r="37" spans="1:14">
+      <c r="A37" s="31"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="14"/>
@@ -1903,9 +2080,9 @@
       <c r="M37" s="15"/>
       <c r="N37" s="12"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="32"/>
+    <row r="38" spans="1:14">
+      <c r="A38" s="31"/>
+      <c r="B38" s="34"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="14"/>
@@ -1919,9 +2096,9 @@
       <c r="M38" s="15"/>
       <c r="N38" s="12"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="29"/>
-      <c r="B39" s="32"/>
+    <row r="39" spans="1:14">
+      <c r="A39" s="31"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="14"/>
@@ -1935,9 +2112,9 @@
       <c r="M39" s="15"/>
       <c r="N39" s="12"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
-      <c r="B40" s="32"/>
+    <row r="40" spans="1:14">
+      <c r="A40" s="31"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="14"/>
@@ -1951,9 +2128,9 @@
       <c r="M40" s="15"/>
       <c r="N40" s="12"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="29"/>
-      <c r="B41" s="32"/>
+    <row r="41" spans="1:14">
+      <c r="A41" s="31"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="14"/>
@@ -1967,9 +2144,9 @@
       <c r="M41" s="15"/>
       <c r="N41" s="12"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="29"/>
-      <c r="B42" s="32"/>
+    <row r="42" spans="1:14">
+      <c r="A42" s="31"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="14"/>
@@ -1983,9 +2160,9 @@
       <c r="M42" s="15"/>
       <c r="N42" s="12"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="29"/>
-      <c r="B43" s="32"/>
+    <row r="43" spans="1:14">
+      <c r="A43" s="31"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="12"/>
       <c r="D43" s="12"/>
       <c r="E43" s="14"/>
@@ -1999,9 +2176,9 @@
       <c r="M43" s="15"/>
       <c r="N43" s="12"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="29"/>
-      <c r="B44" s="32"/>
+    <row r="44" spans="1:14">
+      <c r="A44" s="31"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="14"/>
@@ -2015,9 +2192,9 @@
       <c r="M44" s="15"/>
       <c r="N44" s="12"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="29"/>
-      <c r="B45" s="32"/>
+    <row r="45" spans="1:14">
+      <c r="A45" s="31"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="14"/>
@@ -2031,9 +2208,9 @@
       <c r="M45" s="15"/>
       <c r="N45" s="12"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="29"/>
-      <c r="B46" s="32"/>
+    <row r="46" spans="1:14">
+      <c r="A46" s="31"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="14"/>
@@ -2047,9 +2224,9 @@
       <c r="M46" s="15"/>
       <c r="N46" s="12"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="29"/>
-      <c r="B47" s="32"/>
+    <row r="47" spans="1:14">
+      <c r="A47" s="31"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="14"/>
@@ -2063,9 +2240,9 @@
       <c r="M47" s="15"/>
       <c r="N47" s="12"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="29"/>
-      <c r="B48" s="32"/>
+    <row r="48" spans="1:14">
+      <c r="A48" s="31"/>
+      <c r="B48" s="34"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="14"/>
@@ -2079,9 +2256,9 @@
       <c r="M48" s="15"/>
       <c r="N48" s="12"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="29"/>
-      <c r="B49" s="32"/>
+    <row r="49" spans="1:14">
+      <c r="A49" s="31"/>
+      <c r="B49" s="34"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="14"/>
@@ -2095,9 +2272,9 @@
       <c r="M49" s="15"/>
       <c r="N49" s="12"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="29"/>
-      <c r="B50" s="32"/>
+    <row r="50" spans="1:14">
+      <c r="A50" s="31"/>
+      <c r="B50" s="34"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="14"/>
@@ -2111,9 +2288,9 @@
       <c r="M50" s="15"/>
       <c r="N50" s="12"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="29"/>
-      <c r="B51" s="32"/>
+    <row r="51" spans="1:14">
+      <c r="A51" s="31"/>
+      <c r="B51" s="34"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="14"/>
@@ -2127,9 +2304,9 @@
       <c r="M51" s="15"/>
       <c r="N51" s="12"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="29"/>
-      <c r="B52" s="32"/>
+    <row r="52" spans="1:14">
+      <c r="A52" s="31"/>
+      <c r="B52" s="34"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="14"/>
@@ -2143,9 +2320,9 @@
       <c r="M52" s="15"/>
       <c r="N52" s="12"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="29"/>
-      <c r="B53" s="32"/>
+    <row r="53" spans="1:14">
+      <c r="A53" s="31"/>
+      <c r="B53" s="34"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="14"/>
@@ -2159,9 +2336,9 @@
       <c r="M53" s="15"/>
       <c r="N53" s="12"/>
     </row>
-    <row r="54" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
-      <c r="B54" s="33"/>
+    <row r="54" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A54" s="32"/>
+      <c r="B54" s="35"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="16"/>
@@ -2175,10 +2352,10 @@
       <c r="M54" s="18"/>
       <c r="N54" s="13"/>
     </row>
-    <row r="55" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="28"/>
-      <c r="B56" s="31"/>
+    <row r="55" spans="1:14" ht="15.75" thickBot="1"/>
+    <row r="56" spans="1:14">
+      <c r="A56" s="30"/>
+      <c r="B56" s="33"/>
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="20"/>
@@ -2192,9 +2369,9 @@
       <c r="M56" s="22"/>
       <c r="N56" s="19"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="29"/>
-      <c r="B57" s="32"/>
+    <row r="57" spans="1:14">
+      <c r="A57" s="31"/>
+      <c r="B57" s="34"/>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
       <c r="E57" s="14"/>
@@ -2208,9 +2385,9 @@
       <c r="M57" s="15"/>
       <c r="N57" s="12"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="29"/>
-      <c r="B58" s="32"/>
+    <row r="58" spans="1:14">
+      <c r="A58" s="31"/>
+      <c r="B58" s="34"/>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
       <c r="E58" s="14"/>
@@ -2224,9 +2401,9 @@
       <c r="M58" s="15"/>
       <c r="N58" s="12"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="29"/>
-      <c r="B59" s="32"/>
+    <row r="59" spans="1:14">
+      <c r="A59" s="31"/>
+      <c r="B59" s="34"/>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="14"/>
@@ -2240,9 +2417,9 @@
       <c r="M59" s="15"/>
       <c r="N59" s="12"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="29"/>
-      <c r="B60" s="32"/>
+    <row r="60" spans="1:14">
+      <c r="A60" s="31"/>
+      <c r="B60" s="34"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="14"/>
@@ -2256,9 +2433,9 @@
       <c r="M60" s="15"/>
       <c r="N60" s="12"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="29"/>
-      <c r="B61" s="32"/>
+    <row r="61" spans="1:14">
+      <c r="A61" s="31"/>
+      <c r="B61" s="34"/>
       <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="14"/>
@@ -2272,9 +2449,9 @@
       <c r="M61" s="15"/>
       <c r="N61" s="12"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="29"/>
-      <c r="B62" s="32"/>
+    <row r="62" spans="1:14">
+      <c r="A62" s="31"/>
+      <c r="B62" s="34"/>
       <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="14"/>
@@ -2288,9 +2465,9 @@
       <c r="M62" s="15"/>
       <c r="N62" s="12"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="29"/>
-      <c r="B63" s="32"/>
+    <row r="63" spans="1:14">
+      <c r="A63" s="31"/>
+      <c r="B63" s="34"/>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="14"/>
@@ -2304,9 +2481,9 @@
       <c r="M63" s="15"/>
       <c r="N63" s="12"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="29"/>
-      <c r="B64" s="32"/>
+    <row r="64" spans="1:14">
+      <c r="A64" s="31"/>
+      <c r="B64" s="34"/>
       <c r="C64" s="12"/>
       <c r="D64" s="12"/>
       <c r="E64" s="14"/>
@@ -2320,9 +2497,9 @@
       <c r="M64" s="15"/>
       <c r="N64" s="12"/>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="29"/>
-      <c r="B65" s="32"/>
+    <row r="65" spans="1:14">
+      <c r="A65" s="31"/>
+      <c r="B65" s="34"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
       <c r="E65" s="14"/>
@@ -2336,9 +2513,9 @@
       <c r="M65" s="15"/>
       <c r="N65" s="12"/>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="29"/>
-      <c r="B66" s="32"/>
+    <row r="66" spans="1:14">
+      <c r="A66" s="31"/>
+      <c r="B66" s="34"/>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
       <c r="E66" s="14"/>
@@ -2352,9 +2529,9 @@
       <c r="M66" s="15"/>
       <c r="N66" s="12"/>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="29"/>
-      <c r="B67" s="32"/>
+    <row r="67" spans="1:14">
+      <c r="A67" s="31"/>
+      <c r="B67" s="34"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
       <c r="E67" s="14"/>
@@ -2368,9 +2545,9 @@
       <c r="M67" s="15"/>
       <c r="N67" s="12"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="29"/>
-      <c r="B68" s="32"/>
+    <row r="68" spans="1:14">
+      <c r="A68" s="31"/>
+      <c r="B68" s="34"/>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="14"/>
@@ -2384,9 +2561,9 @@
       <c r="M68" s="15"/>
       <c r="N68" s="12"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="29"/>
-      <c r="B69" s="32"/>
+    <row r="69" spans="1:14">
+      <c r="A69" s="31"/>
+      <c r="B69" s="34"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
       <c r="E69" s="14"/>
@@ -2400,9 +2577,9 @@
       <c r="M69" s="15"/>
       <c r="N69" s="12"/>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="29"/>
-      <c r="B70" s="32"/>
+    <row r="70" spans="1:14">
+      <c r="A70" s="31"/>
+      <c r="B70" s="34"/>
       <c r="C70" s="12"/>
       <c r="D70" s="12"/>
       <c r="E70" s="14"/>
@@ -2416,9 +2593,9 @@
       <c r="M70" s="15"/>
       <c r="N70" s="12"/>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="29"/>
-      <c r="B71" s="32"/>
+    <row r="71" spans="1:14">
+      <c r="A71" s="31"/>
+      <c r="B71" s="34"/>
       <c r="C71" s="12"/>
       <c r="D71" s="12"/>
       <c r="E71" s="14"/>
@@ -2432,9 +2609,9 @@
       <c r="M71" s="15"/>
       <c r="N71" s="12"/>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="29"/>
-      <c r="B72" s="32"/>
+    <row r="72" spans="1:14">
+      <c r="A72" s="31"/>
+      <c r="B72" s="34"/>
       <c r="C72" s="12"/>
       <c r="D72" s="12"/>
       <c r="E72" s="14"/>
@@ -2448,9 +2625,9 @@
       <c r="M72" s="15"/>
       <c r="N72" s="12"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="29"/>
-      <c r="B73" s="32"/>
+    <row r="73" spans="1:14">
+      <c r="A73" s="31"/>
+      <c r="B73" s="34"/>
       <c r="C73" s="12"/>
       <c r="D73" s="12"/>
       <c r="E73" s="14"/>
@@ -2464,9 +2641,9 @@
       <c r="M73" s="15"/>
       <c r="N73" s="12"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="29"/>
-      <c r="B74" s="32"/>
+    <row r="74" spans="1:14">
+      <c r="A74" s="31"/>
+      <c r="B74" s="34"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="14"/>
@@ -2480,9 +2657,9 @@
       <c r="M74" s="15"/>
       <c r="N74" s="12"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="29"/>
-      <c r="B75" s="32"/>
+    <row r="75" spans="1:14">
+      <c r="A75" s="31"/>
+      <c r="B75" s="34"/>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
       <c r="E75" s="14"/>
@@ -2496,9 +2673,9 @@
       <c r="M75" s="15"/>
       <c r="N75" s="12"/>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A76" s="29"/>
-      <c r="B76" s="32"/>
+    <row r="76" spans="1:14">
+      <c r="A76" s="31"/>
+      <c r="B76" s="34"/>
       <c r="C76" s="12"/>
       <c r="D76" s="12"/>
       <c r="E76" s="14"/>
@@ -2512,9 +2689,9 @@
       <c r="M76" s="15"/>
       <c r="N76" s="12"/>
     </row>
-    <row r="77" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="30"/>
-      <c r="B77" s="33"/>
+    <row r="77" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A77" s="32"/>
+      <c r="B77" s="35"/>
       <c r="C77" s="13"/>
       <c r="D77" s="13"/>
       <c r="E77" s="16"/>
@@ -2554,6 +2731,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C44A67B3B57D954BAE559FE843CA0F3B" ma:contentTypeVersion="0" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="fa0ae4ffadfaf6fcc6c2c602ec821808">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3d6ca9f312fcd1c0ab10337cdbdb729">
     <xsd:element name="properties">
@@ -2667,50 +2859,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E1FD49D-F402-44CA-B239-B9C3B2CCC1EF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80C1555C-3F52-4E61-B55F-20AC6C94620E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{80C1555C-3F52-4E61-B55F-20AC6C94620E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF77CE9F-0541-4339-BEE7-F57DAD4FBCC2}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF77CE9F-0541-4339-BEE7-F57DAD4FBCC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E1FD49D-F402-44CA-B239-B9C3B2CCC1EF}"/>
 </file>
</xml_diff>